<commit_message>
Added assertions, data provider and wrote some testcases
</commit_message>
<xml_diff>
--- a/MyProject1_DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/MyProject1_DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smruti\eclipse-workspace\Projects\MyProject1_DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smruti\git\Selenium-Java-Weekend-Project-1\MyProject1_DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D34436E-3A7F-4A09-94CC-74FEAF451635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ABEBF4-FBC9-4D0B-8C8C-105D0931FB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0AEB5DE-C962-462F-8FCD-387883B59EA2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +30,32 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>smruti</t>
+  </si>
+  <si>
+    <t>sahoo</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +405,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C9E932-0B00-481B-9ACA-D40D1AB4AAC8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>751005</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pushing open customer testcases
</commit_message>
<xml_diff>
--- a/MyProject1_DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/MyProject1_DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smruti\git\Selenium-Java-Weekend-Project-1\MyProject1_DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ABEBF4-FBC9-4D0B-8C8C-105D0931FB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D11005-746F-4A17-97A6-28596AEAF5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0AEB5DE-C962-462F-8FCD-387883B59EA2}"/>
+    <workbookView xWindow="4185" yWindow="1365" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A0AEB5DE-C962-462F-8FCD-387883B59EA2}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>firstname</t>
   </si>
@@ -54,6 +55,33 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>rahul</t>
+  </si>
+  <si>
+    <t>tintun</t>
+  </si>
+  <si>
+    <t>lukeworm</t>
+  </si>
+  <si>
+    <t>smart</t>
+  </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>smruti sahoo</t>
   </si>
 </sst>
 </file>
@@ -405,14 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C9E932-0B00-481B-9ACA-D40D1AB4AAC8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -444,6 +473,96 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>751005</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>751005</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>751009</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>751005</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C37D833-95D2-43B5-9683-0B55B2D6C040}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>